<commit_message>
adding some extra coordinates in muni
</commit_message>
<xml_diff>
--- a/data/coordinates_extra_entities.xlsx
+++ b/data/coordinates_extra_entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C0A10A1-C1AB-1944-AF0F-5D8979823CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F221910C-7626-284F-A3C0-E6DE1F85FCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{8032546D-6970-FE4D-A89B-32080BCC4D76}"/>
+    <workbookView xWindow="16080" yWindow="6040" windowWidth="28040" windowHeight="17440" xr2:uid="{8032546D-6970-FE4D-A89B-32080BCC4D76}"/>
   </bookViews>
   <sheets>
     <sheet name="coordinates_extra_entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="111" uniqueCount="83">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="115" uniqueCount="85">
   <si>
     <t>state.abb</t>
   </si>
@@ -274,13 +274,19 @@
   </si>
   <si>
     <t>murphysboro township</t>
+  </si>
+  <si>
+    <t>milton township</t>
+  </si>
+  <si>
+    <t>lisle township</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -414,6 +420,17 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF001D35"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -757,8 +774,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1134,11 +1154,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A051DB-9FA9-364F-99AF-1BFB8A718588}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+    <col min="7" max="7" width="72.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -1912,7 +1938,7 @@
       <c r="F34">
         <v>32.492221999999998</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1932,7 +1958,7 @@
       <c r="F35">
         <v>33.466667000000001</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1952,7 +1978,7 @@
       <c r="F36">
         <v>38.328732000000002</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2254,6 +2280,46 @@
       </c>
       <c r="G51">
         <v>-89.326110999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1749451</v>
+      </c>
+      <c r="E52" s="2">
+        <v>120211</v>
+      </c>
+      <c r="F52" s="3">
+        <v>41.858611000000003</v>
+      </c>
+      <c r="G52" s="2">
+        <v>-88.089444</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1743952</v>
+      </c>
+      <c r="E53" s="2">
+        <v>119045</v>
+      </c>
+      <c r="F53" s="3">
+        <v>41.771667000000001</v>
+      </c>
+      <c r="G53" s="2">
+        <v>-88.088611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>